<commit_message>
added documentation on benchmarking
</commit_message>
<xml_diff>
--- a/retraining_related/Benchmarking sheet.xlsx
+++ b/retraining_related/Benchmarking sheet.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan\Documents\School-stuff\CS\Capstone\SampleImageClassificationRepo\retraining_related\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D80DE6-000F-4914-B422-6BEA78A63C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hyperparams" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hyperparams2" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hyperparams" sheetId="2" r:id="rId2"/>
+    <sheet name="Hyperparams2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -111,30 +120,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Courier New&quot;"/>
     </font>
@@ -144,7 +155,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -154,36 +165,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
@@ -194,11 +212,17 @@
     <xdr:ext cx="2952750" cy="2095500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image11.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -222,11 +246,17 @@
     <xdr:ext cx="3086100" cy="2190750"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="3" name="image7.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -250,11 +280,17 @@
     <xdr:ext cx="3352800" cy="2333625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="4" name="image1.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -278,11 +314,17 @@
     <xdr:ext cx="3571875" cy="2362200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
+        <xdr:cNvPr id="5" name="image12.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -300,7 +342,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -311,11 +353,17 @@
     <xdr:ext cx="3629025" cy="2667000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image6.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -339,11 +387,17 @@
     <xdr:ext cx="4219575" cy="5210175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="3" name="image8.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -367,11 +421,17 @@
     <xdr:ext cx="3486150" cy="2638425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="4" name="image4.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -395,11 +455,17 @@
     <xdr:ext cx="4581525" cy="4238625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="5" name="image2.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -423,11 +489,17 @@
     <xdr:ext cx="3571875" cy="2638425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="6" name="image5.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -451,11 +523,17 @@
     <xdr:ext cx="4162425" cy="4238625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="7" name="image9.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -479,11 +557,17 @@
     <xdr:ext cx="3705225" cy="2771775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
+        <xdr:cNvPr id="8" name="image10.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -507,11 +591,17 @@
     <xdr:ext cx="4010025" cy="4038600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="9" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -525,15 +615,61 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>583603</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>142432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1243435D-5AF8-F435-0825-6D90F4F25563}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8201025"/>
+          <a:ext cx="4774603" cy="3542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -723,26 +859,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="20.25"/>
-    <col customWidth="1" min="9" max="9" width="16.5"/>
-    <col customWidth="1" min="10" max="10" width="17.13"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +913,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -780,10 +921,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1">
         <v>0.91</v>
@@ -795,7 +936,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -803,10 +944,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="D3" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>0.95</v>
@@ -818,7 +959,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -826,10 +967,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="1">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="D4" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1">
         <v>0.91</v>
@@ -841,7 +982,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -849,10 +990,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="1">
-        <v>632.0</v>
+        <v>632</v>
       </c>
       <c r="D5" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1">
         <v>0.97</v>
@@ -864,7 +1005,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -884,7 +1025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -892,10 +1033,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="D7" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1">
         <v>0.9</v>
@@ -907,7 +1048,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -915,10 +1056,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="1">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="D8" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1">
         <v>0.93</v>
@@ -930,7 +1071,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -938,10 +1079,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="1">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="D9" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
         <v>0.91</v>
@@ -953,7 +1094,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -961,10 +1102,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="1">
-        <v>632.0</v>
+        <v>632</v>
       </c>
       <c r="D10" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1">
         <v>0.96</v>
@@ -976,7 +1117,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1135,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1002,10 +1143,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="D12" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1">
         <v>0.93</v>
@@ -1023,7 +1164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1031,10 +1172,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="D13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1">
         <v>0.92</v>
@@ -1046,7 +1187,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1054,10 +1195,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="D14" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1">
         <v>0.88</v>
@@ -1069,7 +1210,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:15">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1077,10 +1218,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>632.0</v>
+        <v>632</v>
       </c>
       <c r="D15" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="G15" s="3">
         <v>0.97</v>
@@ -1092,7 +1233,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1120,22 +1261,22 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="D17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="G17" s="1">
         <v>0.92</v>
       </c>
       <c r="H17" s="1">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="I17" s="1">
         <v>0.91</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1143,10 +1284,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="D18" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="G18" s="1">
         <v>0.94</v>
@@ -1158,7 +1299,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1166,10 +1307,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>193.0</v>
+        <v>193</v>
       </c>
       <c r="D19" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1">
         <v>0.88</v>
@@ -1181,7 +1322,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1189,10 +1330,10 @@
         <v>30</v>
       </c>
       <c r="C20" s="1">
-        <v>685.0</v>
+        <v>685</v>
       </c>
       <c r="D20" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1">
         <v>0.97</v>
@@ -1204,7 +1345,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1224,10 +1365,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:15">
       <c r="B22" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:15">
       <c r="K26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1235,52 +1376,57 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:15">
       <c r="O27" s="1"/>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="44">
+    <row r="44" spans="1:1">
       <c r="A44" s="4"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3">
       <c r="C5" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>